<commit_message>
Done the automation of personal details on profile page
</commit_message>
<xml_diff>
--- a/Mars Standard Tasks.xlsx
+++ b/Mars Standard Tasks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PIPER\source\repos\piper9797\Skillwap_Test3(standard sprint)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PIPER\source\repos\piper9797\Skillwap_Test3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7255B208-455D-4AAA-BBC0-28E5CBD5E1EE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683B3D39-B5D2-48A5-87C4-C4BB08325428}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9398" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9398" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Manual Tasks" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="81">
   <si>
     <t xml:space="preserve">  Task</t>
   </si>
@@ -566,19 +566,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
@@ -595,6 +582,19 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -916,7 +916,7 @@
   </sheetPr>
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
@@ -2344,8 +2344,8 @@
   </sheetPr>
   <dimension ref="A1:V1001"/>
   <sheetViews>
-    <sheetView zoomScale="106" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2357,10 +2357,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="87.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="22"/>
+      <c r="B1" s="33"/>
       <c r="C1" s="3" t="str">
         <f>HYPERLINK("https://drive.google.com/file/d/1YcylO6HB2Z9_NVkgfN0whSU7RGOrN33B/view?usp=sharing","Download docker-compose.yaml ")</f>
         <v xml:space="preserve">Download docker-compose.yaml </v>
@@ -3645,74 +3645,74 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="29" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="29" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="29" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="29" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="29" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="29" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="29" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="29" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="29" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3845,13 +3845,13 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="9" t="s">
@@ -3874,7 +3874,7 @@
       <c r="A29" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="35" t="s">
+      <c r="B29" s="30" t="s">
         <v>37</v>
       </c>
       <c r="C29" s="20"/>
@@ -3883,7 +3883,7 @@
       <c r="A30" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B30" s="35" t="s">
+      <c r="B30" s="30" t="s">
         <v>38</v>
       </c>
       <c r="C30" s="20"/>
@@ -3892,7 +3892,7 @@
       <c r="A31" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="35" t="s">
+      <c r="B31" s="30" t="s">
         <v>39</v>
       </c>
       <c r="C31" s="20"/>
@@ -3901,7 +3901,7 @@
       <c r="A32" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="35" t="s">
+      <c r="B32" s="30" t="s">
         <v>40</v>
       </c>
       <c r="C32" s="20"/>
@@ -3910,7 +3910,7 @@
       <c r="A33" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="35" t="s">
+      <c r="B33" s="30" t="s">
         <v>41</v>
       </c>
       <c r="C33" s="20"/>
@@ -3919,64 +3919,64 @@
       <c r="A34" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="35" t="s">
+      <c r="B34" s="30" t="s">
         <v>43</v>
       </c>
       <c r="C34" s="20"/>
     </row>
     <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="34" t="s">
+      <c r="A35" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="B35" s="34" t="s">
+      <c r="B35" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C35" s="34"/>
+      <c r="C35" s="29"/>
     </row>
     <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="36" t="s">
+      <c r="A36" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="34" t="s">
+      <c r="B36" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="34"/>
+      <c r="C36" s="29"/>
     </row>
     <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="36" t="s">
+      <c r="A37" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="B37" s="34" t="s">
+      <c r="B37" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="C37" s="34"/>
+      <c r="C37" s="29"/>
     </row>
     <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="36" t="s">
+      <c r="A38" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="34" t="s">
+      <c r="B38" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="C38" s="34"/>
+      <c r="C38" s="29"/>
     </row>
     <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="36" t="s">
+      <c r="A39" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="B39" s="34" t="s">
+      <c r="B39" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C39" s="34"/>
+      <c r="C39" s="29"/>
     </row>
     <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="36" t="s">
+      <c r="A40" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="B40" s="34" t="s">
+      <c r="B40" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="C40" s="34"/>
+      <c r="C40" s="29"/>
     </row>
     <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4975,11 +4975,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
@@ -5005,7 +5005,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="22" t="s">
         <v>50</v>
       </c>
       <c r="B3" s="14" t="s">
@@ -5016,7 +5016,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="22" t="s">
         <v>53</v>
       </c>
       <c r="B4" s="15" t="s">
@@ -5027,7 +5027,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="23" t="s">
         <v>61</v>
       </c>
       <c r="B5" s="15" t="s">
@@ -5038,7 +5038,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="23" t="s">
         <v>62</v>
       </c>
       <c r="B6" s="15" t="s">
@@ -5049,7 +5049,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="26" t="s">
         <v>63</v>
       </c>
       <c r="B7" s="15" t="s">
@@ -5058,12 +5058,12 @@
       <c r="C7" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="21" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="26" t="s">
         <v>65</v>
       </c>
       <c r="B8" s="15" t="s">
@@ -5072,12 +5072,12 @@
       <c r="C8" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="F8" s="29" t="s">
+      <c r="F8" s="24" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="26" t="s">
         <v>67</v>
       </c>
       <c r="B9" s="15" t="s">
@@ -5086,12 +5086,12 @@
       <c r="C9" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="F9" s="29" t="s">
+      <c r="F9" s="24" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="25" t="s">
         <v>68</v>
       </c>
       <c r="B10" s="15" t="s">
@@ -5102,7 +5102,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="26" t="s">
         <v>69</v>
       </c>
       <c r="B11" s="15" t="s">
@@ -5111,12 +5111,12 @@
       <c r="C11" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="32" t="s">
+      <c r="F11" s="27" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="26" t="s">
         <v>71</v>
       </c>
       <c r="B12" s="15" t="s">
@@ -5125,12 +5125,12 @@
       <c r="C12" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="F12" s="32" t="s">
+      <c r="F12" s="27" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="26" t="s">
         <v>72</v>
       </c>
       <c r="B13" s="15" t="s">
@@ -5139,7 +5139,7 @@
       <c r="C13" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="F13" s="32" t="s">
+      <c r="F13" s="27" t="s">
         <v>70</v>
       </c>
     </row>
@@ -5156,7 +5156,7 @@
       <c r="F14" s="17"/>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="22" t="s">
         <v>56</v>
       </c>
       <c r="B15" s="15" t="s">
@@ -5165,7 +5165,7 @@
       <c r="C15" s="18"/>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="23" t="s">
         <v>73</v>
       </c>
       <c r="B16" s="15" t="s">
@@ -5174,55 +5174,55 @@
       <c r="C16" s="18"/>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="28" t="s">
         <v>74</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>57</v>
       </c>
       <c r="C17" s="18"/>
-      <c r="F17" s="26" t="s">
+      <c r="F17" s="21" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="33" t="s">
+      <c r="A18" s="28" t="s">
         <v>76</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>57</v>
       </c>
       <c r="C18" s="18"/>
-      <c r="F18" s="29" t="s">
+      <c r="F18" s="24" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="28" t="s">
         <v>78</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>57</v>
       </c>
       <c r="C19" s="18"/>
-      <c r="F19" s="29" t="s">
+      <c r="F19" s="24" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="33" t="s">
+      <c r="A20" s="28" t="s">
         <v>79</v>
       </c>
       <c r="B20" s="15" t="s">
         <v>57</v>
       </c>
       <c r="C20" s="18"/>
-      <c r="F20" s="26" t="s">
+      <c r="F20" s="21" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="23" t="s">
         <v>80</v>
       </c>
       <c r="B21" s="15" t="s">

</xml_diff>

<commit_message>
Done the automation testing for profile_page
</commit_message>
<xml_diff>
--- a/Mars Standard Tasks.xlsx
+++ b/Mars Standard Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PIPER\source\repos\piper9797\Skillwap_Test3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683B3D39-B5D2-48A5-87C4-C4BB08325428}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F882F2-EDE5-4AEE-A18A-DC11F911864D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9398" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="84">
   <si>
     <t xml:space="preserve">  Task</t>
   </si>
@@ -298,6 +298,18 @@
   </si>
   <si>
     <t>http://www.dneonline.com/calculator.asmx?WSDL</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Profile --&gt; Skills</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Profile --&gt; Loc, Availability, Hours, Earn Target</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Manage Listings --&gt; Edit </t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
 </sst>
@@ -540,7 +552,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -596,6 +608,9 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -917,7 +932,7 @@
   <dimension ref="A1:Y1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2345,7 +2360,7 @@
   <dimension ref="A1:V1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2417,40 +2432,40 @@
       <c r="V2" s="5"/>
     </row>
     <row r="3" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="37" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="37" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="20" t="s">
+      <c r="A5" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="37" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="37" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="20" t="s">
-        <v>13</v>
+      <c r="A7" s="38" t="s">
+        <v>81</v>
       </c>
       <c r="B7" s="20" t="s">
         <v>9</v>
@@ -2473,10 +2488,10 @@
       </c>
     </row>
     <row r="10" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="37" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2497,8 +2512,8 @@
       </c>
     </row>
     <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="20" t="s">
-        <v>19</v>
+      <c r="A13" s="38" t="s">
+        <v>83</v>
       </c>
       <c r="B13" s="20" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Finish "add education" and "add certifications" in the profile page
</commit_message>
<xml_diff>
--- a/Mars Standard Tasks.xlsx
+++ b/Mars Standard Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PIPER\source\repos\piper9797\Skillwap_Test3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F882F2-EDE5-4AEE-A18A-DC11F911864D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E17217A-55A5-4E9E-A1B0-7D597FEB9185}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9398" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9398" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Manual Tasks" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="86">
   <si>
     <t xml:space="preserve">  Task</t>
   </si>
@@ -310,6 +310,14 @@
   </si>
   <si>
     <t xml:space="preserve">Manage Listings --&gt; Edit </t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Profile --&gt; Languages</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sanity Test Cases</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
 </sst>
@@ -931,8 +939,8 @@
   </sheetPr>
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -983,10 +991,10 @@
       <c r="Y1" s="7"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="37" t="s">
         <v>8</v>
       </c>
     </row>
@@ -999,98 +1007,98 @@
       </c>
     </row>
     <row r="4" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="37" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="37" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="37" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="37" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="A8" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="37" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="A9" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="37" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="A10" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="37" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="A11" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="37" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="A12" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="37" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="A13" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="37" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="A14" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="37" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="A15" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="37" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1206,98 +1214,98 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+      <c r="A30" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="37" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+      <c r="A31" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="37" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+      <c r="A32" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="37" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+      <c r="A33" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="37" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+      <c r="A34" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="37" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+      <c r="A35" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="37" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+      <c r="A36" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="37" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+      <c r="A37" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="37" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+      <c r="A38" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="37" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+      <c r="A39" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="37" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+      <c r="A40" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="37" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+      <c r="A41" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="37" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2360,7 +2368,7 @@
   <dimension ref="A1:V1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2456,8 +2464,8 @@
       </c>
     </row>
     <row r="6" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="37" t="s">
-        <v>12</v>
+      <c r="A6" s="39" t="s">
+        <v>84</v>
       </c>
       <c r="B6" s="37" t="s">
         <v>9</v>
@@ -2624,8 +2632,8 @@
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="20" t="s">
-        <v>33</v>
+      <c r="A27" s="38" t="s">
+        <v>85</v>
       </c>
       <c r="B27" s="20" t="s">
         <v>9</v>
@@ -3631,7 +3639,7 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Done all the automation tasks
</commit_message>
<xml_diff>
--- a/Mars Standard Tasks.xlsx
+++ b/Mars Standard Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PIPER\source\repos\piper9797\Skillwap_Test3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E17217A-55A5-4E9E-A1B0-7D597FEB9185}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA27256-A88A-4729-AA2F-FA044AF490AB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9398" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9398" tabRatio="970" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Manual Tasks" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="91">
   <si>
     <t xml:space="preserve">  Task</t>
   </si>
@@ -216,10 +216,6 @@
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
   <si>
-    <t>11th</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
     <t>Registration</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
@@ -318,6 +314,30 @@
   </si>
   <si>
     <t>Sanity Test Cases</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Selenium Task</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>(Just one public account which I canot change the password)</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>selenium Task</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>(the result cannot save after editing)</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Manage Request --&gt; Received Request</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Search Skills --&gt; by Filters</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
 </sst>
@@ -603,6 +623,9 @@
     <xf numFmtId="0" fontId="15" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -616,9 +639,6 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -939,8 +959,8 @@
   </sheetPr>
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -991,10 +1011,10 @@
       <c r="Y1" s="7"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="32" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1007,98 +1027,98 @@
       </c>
     </row>
     <row r="4" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="32" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="32" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="32" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="32" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="32" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="32" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="32" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="32" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="32" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="32" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="32" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="32" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1214,98 +1234,98 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="37" t="s">
+      <c r="A30" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="37" t="s">
+      <c r="B30" s="32" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="37" t="s">
+      <c r="A31" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="37" t="s">
+      <c r="B31" s="32" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="37" t="s">
+      <c r="A32" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="37" t="s">
+      <c r="B32" s="32" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="37" t="s">
+      <c r="B33" s="32" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="37" t="s">
+      <c r="A34" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B34" s="37" t="s">
+      <c r="B34" s="32" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="37" t="s">
+      <c r="A35" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B35" s="37" t="s">
+      <c r="B35" s="32" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="37" t="s">
+      <c r="A36" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B36" s="37" t="s">
+      <c r="B36" s="32" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="37" t="s">
+      <c r="A37" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="B37" s="37" t="s">
+      <c r="B37" s="32" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="37" t="s">
+      <c r="A38" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="B38" s="37" t="s">
+      <c r="B38" s="32" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="37" t="s">
+      <c r="A39" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B39" s="37" t="s">
+      <c r="B39" s="32" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="37" t="s">
+      <c r="A40" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="B40" s="37" t="s">
+      <c r="B40" s="32" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="37" t="s">
+      <c r="A41" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="B41" s="37" t="s">
+      <c r="B41" s="32" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2367,23 +2387,23 @@
   </sheetPr>
   <dimension ref="A1:V1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="106" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="43.73046875" customWidth="1"/>
     <col min="2" max="2" width="36.1328125" customWidth="1"/>
-    <col min="3" max="3" width="30.73046875" customWidth="1"/>
+    <col min="3" max="3" width="43.73046875" customWidth="1"/>
     <col min="4" max="4" width="39" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="87.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="33"/>
+      <c r="B1" s="36"/>
       <c r="C1" s="3" t="str">
         <f>HYPERLINK("https://drive.google.com/file/d/1YcylO6HB2Z9_NVkgfN0whSU7RGOrN33B/view?usp=sharing","Download docker-compose.yaml ")</f>
         <v xml:space="preserve">Download docker-compose.yaml </v>
@@ -2440,67 +2460,67 @@
       <c r="V2" s="5"/>
     </row>
     <row r="3" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="32" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="32" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="39" t="s">
-        <v>82</v>
-      </c>
-      <c r="B5" s="37" t="s">
+      <c r="A5" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="32" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="39" t="s">
-        <v>84</v>
-      </c>
-      <c r="B6" s="37" t="s">
+      <c r="A6" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="32" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="38" t="s">
-        <v>81</v>
-      </c>
-      <c r="B7" s="20" t="s">
+      <c r="A7" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="32" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="32" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="32" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="37" t="s">
-        <v>9</v>
+      <c r="B10" s="34" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2510,60 +2530,66 @@
       <c r="B11" s="20" t="s">
         <v>9</v>
       </c>
+      <c r="C11" s="21" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="12" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="32" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="38" t="s">
-        <v>83</v>
-      </c>
-      <c r="B13" s="20" t="s">
+      <c r="A13" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="32" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="20" t="s">
+    <row r="15" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" s="32" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="20" t="s">
+    <row r="16" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="32" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="20" t="s">
+    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="32" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>9</v>
-      </c>
-    </row>
     <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="20" t="s">
+      <c r="A18" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18" s="32" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2632,8 +2658,8 @@
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="38" t="s">
-        <v>85</v>
+      <c r="A27" s="33" t="s">
+        <v>84</v>
       </c>
       <c r="B27" s="20" t="s">
         <v>9</v>
@@ -2642,9 +2668,7 @@
     <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="20" t="s">
-        <v>59</v>
-      </c>
+      <c r="A30" s="20"/>
     </row>
     <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3639,8 +3663,8 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3669,7 +3693,7 @@
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>7</v>
@@ -3868,13 +3892,13 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="34" t="s">
+      <c r="A27" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="35"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="9" t="s">
@@ -4986,7 +5010,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4998,11 +5022,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
@@ -5051,7 +5075,7 @@
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>51</v>
@@ -5062,7 +5086,7 @@
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>51</v>
@@ -5073,7 +5097,7 @@
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>51</v>
@@ -5082,12 +5106,12 @@
         <v>54</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>51</v>
@@ -5096,12 +5120,12 @@
         <v>54</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>51</v>
@@ -5110,12 +5134,12 @@
         <v>54</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B10" s="15" t="s">
         <v>51</v>
@@ -5126,7 +5150,7 @@
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>51</v>
@@ -5135,12 +5159,12 @@
         <v>54</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>51</v>
@@ -5149,12 +5173,12 @@
         <v>54</v>
       </c>
       <c r="F12" s="27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>51</v>
@@ -5163,7 +5187,7 @@
         <v>54</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5189,7 +5213,7 @@
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>57</v>
@@ -5198,55 +5222,55 @@
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>57</v>
       </c>
       <c r="C17" s="18"/>
       <c r="F17" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>57</v>
       </c>
       <c r="C18" s="18"/>
       <c r="F18" s="24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>57</v>
       </c>
       <c r="C19" s="18"/>
       <c r="F19" s="24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B20" s="15" t="s">
         <v>57</v>
       </c>
       <c r="C20" s="18"/>
       <c r="F20" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B21" s="15" t="s">
         <v>57</v>

</xml_diff>

<commit_message>
Fixed some format problems
</commit_message>
<xml_diff>
--- a/Mars Standard Tasks.xlsx
+++ b/Mars Standard Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PIPER\source\repos\piper9797\Skillwap_Test3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA27256-A88A-4729-AA2F-FA044AF490AB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0A7D01-0D65-4A35-8502-7CDC027299E4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9398" tabRatio="970" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="3818" tabRatio="970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Manual Tasks" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="100">
   <si>
     <t xml:space="preserve">  Task</t>
   </si>
@@ -133,9 +133,6 @@
   </si>
   <si>
     <t>Sanity Test Cases</t>
-  </si>
-  <si>
-    <t>Manual Test Case</t>
   </si>
   <si>
     <t>Performance Testing Tasks</t>
@@ -338,6 +335,46 @@
   </si>
   <si>
     <t>Search Skills --&gt; by Filters</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Notifications --&gt; Select one notification</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Notifications --&gt; See All&amp;Select All&amp;Mark as Read</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>have no histry button</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>have no job scheduler</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>have no new functions</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Search Skills --&gt; by All Categories, Sub Categories</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Notifications --&gt; See all</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Job Scheduler</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Manual Test Condition     have no job scheduler</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Manual Test Condition     have no new functions</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
 </sst>
@@ -580,7 +617,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -593,7 +630,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -957,15 +993,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Y1000"/>
+  <dimension ref="A1:Y972"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="41.1328125" customWidth="1"/>
+    <col min="1" max="1" width="62.06640625" customWidth="1"/>
     <col min="2" max="2" width="55.1328125" customWidth="1"/>
     <col min="3" max="3" width="18.73046875" customWidth="1"/>
     <col min="4" max="4" width="22.86328125" customWidth="1"/>
@@ -1011,424 +1047,231 @@
       <c r="Y1" s="7"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="31" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="31" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="31" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="31" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="31" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="31" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="31" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="31" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="31" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="31" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="31" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="31" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="31" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="31" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="A16" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="B16" s="31" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="31" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" t="s">
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" s="31" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="31" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" t="s">
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="31" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" t="s">
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="31" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="C23" s="20"/>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
         <v>33</v>
       </c>
-      <c r="B26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>5</v>
-      </c>
-      <c r="B28" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>10</v>
-      </c>
-      <c r="B29" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="B30" s="32" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="B31" s="32" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="B32" s="32" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="B33" s="32" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="B34" s="32" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="B35" s="32" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="B36" s="32" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="B37" s="32" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="B38" s="32" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="B39" s="32" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="B40" s="32" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="B41" s="32" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>23</v>
-      </c>
-      <c r="B42" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>24</v>
-      </c>
-      <c r="B43" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>25</v>
-      </c>
-      <c r="B44" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>26</v>
-      </c>
-      <c r="B45" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>27</v>
-      </c>
-      <c r="B46" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>28</v>
-      </c>
-      <c r="B47" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>29</v>
-      </c>
-      <c r="B48" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>30</v>
-      </c>
-      <c r="B49" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>31</v>
-      </c>
-      <c r="B50" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>32</v>
-      </c>
-      <c r="B51" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>33</v>
-      </c>
-      <c r="B52" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="54" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="55" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="56" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="57" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="58" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="59" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="60" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="61" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="62" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="63" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="64" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+      <c r="B24" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" s="20"/>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2337,41 +2180,13 @@
     <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <phoneticPr fontId="13" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" sqref="B1:B26 B28:B52 B67:B1000" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="B39:B972 B1:B24" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Manual Test Condition,Manual Test Case,Selenium Task,Specflow Task,Performance Testing Task"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="E1:E26 E28:E52 E67:E1000" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" sqref="E39:E972 E1:E24" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Not Yet assigned,In-Progress,Done"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2385,10 +2200,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:V1001"/>
+  <dimension ref="A1:V998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="106" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="A10" zoomScale="106" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2400,10 +2215,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="87.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" s="36"/>
+      <c r="A1" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="35"/>
       <c r="C1" s="3" t="str">
         <f>HYPERLINK("https://drive.google.com/file/d/1YcylO6HB2Z9_NVkgfN0whSU7RGOrN33B/view?usp=sharing","Download docker-compose.yaml ")</f>
         <v xml:space="preserve">Download docker-compose.yaml </v>
@@ -2432,10 +2247,10 @@
       <c r="V1" s="5"/>
     </row>
     <row r="2" spans="1:22" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="5"/>
@@ -2460,218 +2275,206 @@
       <c r="V2" s="5"/>
     </row>
     <row r="3" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="31" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="31" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B13" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="31" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="34" t="s">
+    <row r="15" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" s="31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="B20" s="31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B24" s="19" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="34" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" s="32" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="32" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="32" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="34" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="32" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="B13" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="32" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="34" t="s">
-        <v>89</v>
-      </c>
-      <c r="B15" s="32" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="32" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="32" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="34" t="s">
-        <v>90</v>
-      </c>
-      <c r="B18" s="32" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" s="20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23" s="20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="33" t="s">
-        <v>84</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="20"/>
-    </row>
-    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+      <c r="C24" s="20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="19"/>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3638,16 +3441,13 @@
     <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="B2:B27" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="B2:B24" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Manual Test Condition,Manual Test Case,Selenium Task,Specflow Task,Performance Testing Task"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3663,8 +3463,8 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3692,338 +3492,338 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" s="29" t="s">
+      <c r="A2" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="28" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="28" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="28" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="28" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="28" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="28" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="28" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="28" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="28" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="38"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="20" t="s">
+      <c r="B29" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="30" t="s">
+      <c r="C29" s="19"/>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="20"/>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="20" t="s">
+      <c r="C30" s="19"/>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="19"/>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="19"/>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="19"/>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" s="19"/>
+    </row>
+    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="B30" s="30" t="s">
+      <c r="C35" s="28"/>
+    </row>
+    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" s="28"/>
+    </row>
+    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="20"/>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="B31" s="30" t="s">
+      <c r="C37" s="28"/>
+    </row>
+    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="C31" s="20"/>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32" s="30" t="s">
+      <c r="C38" s="28"/>
+    </row>
+    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="C32" s="20"/>
-    </row>
-    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="B33" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="C33" s="20"/>
-    </row>
-    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="20" t="s">
+      <c r="C39" s="28"/>
+    </row>
+    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="B40" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="C34" s="20"/>
-    </row>
-    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="B35" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="C35" s="29"/>
-    </row>
-    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="B36" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="C36" s="29"/>
-    </row>
-    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="B37" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="C37" s="29"/>
-    </row>
-    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="B38" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="C38" s="29"/>
-    </row>
-    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="B39" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="C39" s="29"/>
-    </row>
-    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="B40" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="C40" s="29"/>
+      <c r="C40" s="28"/>
     </row>
     <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -5022,273 +4822,273 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+    </row>
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-    </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="D2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="22" t="s">
+      <c r="B3" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="C3" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="15" t="s">
+    </row>
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="21" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="22" t="s">
+      <c r="B4" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="23" t="s">
+    </row>
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="15" t="s">
+      <c r="B7" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="10" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="F7" s="21" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="F8" s="24" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="F11" s="27" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="F12" s="27" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="26" t="s">
+      <c r="B14" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="15"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+    </row>
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="17"/>
+    </row>
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="F13" s="27" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-    </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="22" t="s">
+      <c r="B16" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" s="18"/>
-    </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="23" t="s">
+      <c r="C16" s="17"/>
+    </row>
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="B16" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="C16" s="18"/>
-    </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="28" t="s">
+      <c r="B17" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="17"/>
+      <c r="F17" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="B17" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="C17" s="18"/>
-      <c r="F17" s="21" t="s">
+    </row>
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="27" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="28" t="s">
+      <c r="B18" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="17"/>
+      <c r="F18" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="B18" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="C18" s="18"/>
-      <c r="F18" s="24" t="s">
+    </row>
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="27" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="28" t="s">
+      <c r="B19" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="17"/>
+      <c r="F19" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="18"/>
-      <c r="F19" s="24" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="28" t="s">
+      <c r="B20" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="17"/>
+      <c r="F20" s="20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="B20" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20" s="18"/>
-      <c r="F20" s="21" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="18"/>
+      <c r="B21" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="17"/>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="11"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
+      <c r="A22" s="10"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="13"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="18"/>
+      <c r="A23" s="12"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Done all the specflow
</commit_message>
<xml_diff>
--- a/Mars Standard Tasks.xlsx
+++ b/Mars Standard Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PIPER\source\repos\piper9797\Skillwap_Test3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0A7D01-0D65-4A35-8502-7CDC027299E4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03980884-8918-4861-AE67-08ABA653BE55}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="3818" tabRatio="970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="3818" tabRatio="970" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Manual Tasks" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="100">
   <si>
     <t xml:space="preserve">  Task</t>
   </si>
@@ -995,8 +995,8 @@
   </sheetPr>
   <dimension ref="A1:Y972"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1207,10 +1207,10 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="A22" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="31" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3463,7 +3463,7 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Done the performance testing
</commit_message>
<xml_diff>
--- a/Mars Standard Tasks.xlsx
+++ b/Mars Standard Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PIPER\source\repos\piper9797\Skillwap_Test3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03980884-8918-4861-AE67-08ABA653BE55}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742295C2-D6B3-45BA-991F-F7DB47D3B956}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="3818" tabRatio="970" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="105">
   <si>
     <t xml:space="preserve">  Task</t>
   </si>
@@ -106,12 +106,6 @@
   </si>
   <si>
     <t>Search Skills --&gt; by Filters</t>
-  </si>
-  <si>
-    <t>Notifications --&gt; Show Less</t>
-  </si>
-  <si>
-    <t>Notifications --&gt; Load more</t>
   </si>
   <si>
     <t xml:space="preserve">Notifications --&gt; Delete </t>
@@ -375,6 +369,34 @@
   </si>
   <si>
     <t>Manual Test Condition     have no new functions</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Profile --&gt; Loc, Availability, Hours, Earn Target</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Search Skills --&gt; by All Categories, Sub Categories</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Manage Request --&gt; Received Request</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Manage Request --&gt; Sent Request</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Share Skills --&gt; Add New</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Manage Listings --&gt; Edit </t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Profile --&gt; Languages</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
 </sst>
@@ -1160,7 +1182,7 @@
     </row>
     <row r="16" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="33" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B16" s="31" t="s">
         <v>8</v>
@@ -1176,7 +1198,7 @@
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="33" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B18" s="31" t="s">
         <v>8</v>
@@ -1184,7 +1206,7 @@
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="31" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B19" s="31" t="s">
         <v>8</v>
@@ -1192,7 +1214,7 @@
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="31" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B20" s="31" t="s">
         <v>8</v>
@@ -1200,7 +1222,7 @@
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="31" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B21" s="31" t="s">
         <v>8</v>
@@ -1208,7 +1230,7 @@
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="31" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B22" s="31" t="s">
         <v>8</v>
@@ -1216,19 +1238,19 @@
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C23" s="20"/>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C24" s="20"/>
     </row>
@@ -2202,8 +2224,8 @@
   </sheetPr>
   <dimension ref="A1:V998"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="106" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView topLeftCell="A7" zoomScale="106" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2216,7 +2238,7 @@
   <sheetData>
     <row r="1" spans="1:22" ht="87.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="34" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B1" s="35"/>
       <c r="C1" s="3" t="str">
@@ -2292,7 +2314,7 @@
     </row>
     <row r="5" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="33" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B5" s="31" t="s">
         <v>9</v>
@@ -2300,7 +2322,7 @@
     </row>
     <row r="6" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="33" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B6" s="31" t="s">
         <v>9</v>
@@ -2308,7 +2330,7 @@
     </row>
     <row r="7" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="33" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B7" s="31" t="s">
         <v>9</v>
@@ -2335,7 +2357,7 @@
         <v>16</v>
       </c>
       <c r="B10" s="33" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2346,7 +2368,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2359,13 +2381,13 @@
     </row>
     <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="33" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2378,7 +2400,7 @@
     </row>
     <row r="15" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="33" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B15" s="31" t="s">
         <v>9</v>
@@ -2402,7 +2424,7 @@
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="33" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B18" s="31" t="s">
         <v>9</v>
@@ -2410,7 +2432,7 @@
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="33" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B19" s="31" t="s">
         <v>9</v>
@@ -2418,7 +2440,7 @@
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="33" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B20" s="31" t="s">
         <v>9</v>
@@ -2426,7 +2448,7 @@
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="31" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B21" s="31" t="s">
         <v>9</v>
@@ -2434,35 +2456,35 @@
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B22" s="19" t="s">
         <v>9</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B23" s="19" t="s">
         <v>9</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="32" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B24" s="19" t="s">
         <v>9</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3461,17 +3483,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E1000"/>
+  <dimension ref="A1:E996"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="50.73046875" customWidth="1"/>
     <col min="2" max="2" width="27.53125" customWidth="1"/>
-    <col min="3" max="6" width="14.3984375" customWidth="1"/>
+    <col min="3" max="3" width="25.9296875" customWidth="1"/>
+    <col min="4" max="6" width="14.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -3493,7 +3516,7 @@
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="28" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B2" s="28" t="s">
         <v>7</v>
@@ -3509,7 +3532,7 @@
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="28" t="s">
-        <v>11</v>
+        <v>98</v>
       </c>
       <c r="B4" s="28" t="s">
         <v>7</v>
@@ -3517,7 +3540,7 @@
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="28" t="s">
-        <v>12</v>
+        <v>104</v>
       </c>
       <c r="B5" s="28" t="s">
         <v>7</v>
@@ -3562,18 +3585,21 @@
       <c r="B10" s="28" t="s">
         <v>7</v>
       </c>
+      <c r="C10" s="20" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="19" t="s">
-        <v>18</v>
+      <c r="A11" s="32" t="s">
+        <v>102</v>
       </c>
       <c r="B11" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="19" t="s">
-        <v>19</v>
+      <c r="A12" s="32" t="s">
+        <v>103</v>
       </c>
       <c r="B12" s="19" t="s">
         <v>7</v>
@@ -3589,23 +3615,23 @@
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="19" t="s">
-        <v>21</v>
+        <v>100</v>
       </c>
       <c r="B14" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="19" t="s">
-        <v>22</v>
+      <c r="A15" s="32" t="s">
+        <v>101</v>
       </c>
       <c r="B15" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="19" t="s">
-        <v>23</v>
+      <c r="A16" s="32" t="s">
+        <v>99</v>
       </c>
       <c r="B16" s="19" t="s">
         <v>7</v>
@@ -3620,24 +3646,24 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="19" t="s">
-        <v>25</v>
+      <c r="A18" s="32" t="s">
+        <v>89</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="19" t="s">
-        <v>26</v>
+      <c r="A19" s="32" t="s">
+        <v>88</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="19" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B20" s="19" t="s">
         <v>7</v>
@@ -3645,186 +3671,164 @@
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="19" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B21" s="19" t="s">
         <v>7</v>
       </c>
+      <c r="C21" s="20" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="19" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B22" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24" s="19" t="s">
-        <v>7</v>
+      <c r="C22" s="20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" s="19" t="s">
-        <v>7</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="B25" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="19"/>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="B26" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="19"/>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="19"/>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="19"/>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C29" s="19"/>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="19"/>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="28"/>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="29" t="s">
+      <c r="C32" s="28"/>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="28"/>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="19"/>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B31" s="29" t="s">
+      <c r="C34" s="28"/>
+    </row>
+    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35" s="28" t="s">
         <v>38</v>
-      </c>
-      <c r="C31" s="19"/>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B32" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="C32" s="19"/>
-    </row>
-    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B33" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="C33" s="19"/>
-    </row>
-    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="B34" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="C34" s="19"/>
-    </row>
-    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="B35" s="28" t="s">
-        <v>36</v>
       </c>
       <c r="C35" s="28"/>
     </row>
     <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="30" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B36" s="28" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C36" s="28"/>
     </row>
-    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="B37" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="C37" s="28"/>
-    </row>
-    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="B38" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="C38" s="28"/>
-    </row>
-    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="B39" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="C39" s="28"/>
-    </row>
-    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="B40" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="C40" s="28"/>
-    </row>
+    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4781,24 +4785,21 @@
     <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="A23:E23"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" sqref="B1:B26 B29:B40" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="B25:B36 B1:B22" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Manual Test Condition,Manual Test Case,Selenium Task,Specflow Task,Performance Testing Task"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="E1:E26 E29:E40" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="list" allowBlank="1" sqref="E25:E36 E1:E22" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"Not Yet assigned,In-Progress,Done"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4823,7 +4824,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="38" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="37"/>
@@ -4833,13 +4834,13 @@
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>46</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>48</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>3</v>
@@ -4853,149 +4854,149 @@
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>49</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="22" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="25" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="25" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="24" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="25" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F11" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="25" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F12" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="25" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F13" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="16"/>
@@ -5004,76 +5005,76 @@
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C15" s="17"/>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C16" s="17"/>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C17" s="17"/>
       <c r="F17" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C18" s="17"/>
       <c r="F18" s="23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="27" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C19" s="17"/>
       <c r="F19" s="23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="27" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C20" s="17"/>
       <c r="F20" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C21" s="17"/>
     </row>

</xml_diff>